<commit_message>
Update files to latest version
</commit_message>
<xml_diff>
--- a/automotive_domain_outcomes.xlsx
+++ b/automotive_domain_outcomes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="468">
   <si>
     <t>P</t>
   </si>
@@ -515,7 +515,24 @@
     <t>f_1</t>
   </si>
   <si>
-    <t>embrace(p_13, p_75)</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Abuse of authorisations </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(embrace(p_13, p_75))</t>
   </si>
   <si>
     <t>f_2</t>
@@ -554,13 +571,44 @@
     <t>f_7</t>
   </si>
   <si>
-    <t>embrace(p_20, p_32)</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Communication protocol hijacking </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in car devices</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(embrace(p_20, p_32))</t>
   </si>
   <si>
     <t>f_8</t>
   </si>
   <si>
-    <t>Data Aggregation and Profiling</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Data aggregation and profiling </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>of driver</t>
+    </r>
   </si>
   <si>
     <t>rename(embrace(p_39, p_49, p_50))</t>
@@ -569,7 +617,24 @@
     <t>f_9</t>
   </si>
   <si>
-    <t>embrace(p_71, p_1)</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Data loss </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(embrace(p_71, p_1))</t>
   </si>
   <si>
     <t>f_10</t>
@@ -584,10 +649,44 @@
     <t>f_13</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Failure to meet contractual requirements </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>with driver</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_27)</t>
+  </si>
+  <si>
     <t>f_14</t>
   </si>
   <si>
-    <t>Failures or sabotage</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Failures or sabotage </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>of car components</t>
+    </r>
   </si>
   <si>
     <t>rename(embrace(p_7, p_9, p_14, p_19))</t>
@@ -602,9 +701,32 @@
     <t>f_16</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Identity theft </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>of driver</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_12)</t>
+  </si>
+  <si>
     <t>f_17</t>
   </si>
   <si>
+    <t>Infotainment alteration</t>
+  </si>
+  <si>
     <t>embrace(p_73, p_3, p_37, p_43, p_44)</t>
   </si>
   <si>
@@ -626,28 +748,77 @@
     <t>f_21</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Man-in-the-middle attack / Session hijacking </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_22)</t>
+  </si>
+  <si>
     <t>f_22</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Manipulation of information </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_4)</t>
+  </si>
+  <si>
     <t>f_23</t>
   </si>
   <si>
+    <t>Mobile app malware</t>
+  </si>
+  <si>
     <t>embrace(p_57, p_2)</t>
   </si>
   <si>
     <t>f_24</t>
   </si>
   <si>
+    <t>Mobile app spoofing</t>
+  </si>
+  <si>
     <t>embrace(p_51, p_3, p_39)</t>
   </si>
   <si>
     <t>f_25</t>
   </si>
   <si>
+    <t>OEM targeted attacks</t>
+  </si>
+  <si>
     <t>f_26</t>
   </si>
   <si>
-    <t>Server information leakage</t>
+    <t>OEM servers information leakage</t>
   </si>
   <si>
     <t>rename(p_24)</t>
@@ -656,9 +827,49 @@
     <t>f_27</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Servers violation </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_67)</t>
+  </si>
+  <si>
     <t>f_28</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Side-channel attacks </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>against car components</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_16)</t>
+  </si>
+  <si>
     <t>f_29</t>
   </si>
   <si>
@@ -677,7 +888,21 @@
     <t>f_32</t>
   </si>
   <si>
-    <t>Software Vulnerabilities Exploitation</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Software vulnerabilities exploitation </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
   </si>
   <si>
     <t>rename(embrace(p_18, p_33, p_36, p_38, p_46, p_65))</t>
@@ -686,6 +911,26 @@
     <t>f_33</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Theft </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>of car</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_15)</t>
+  </si>
+  <si>
     <t>f_34</t>
   </si>
   <si>
@@ -695,16 +940,47 @@
     <t>f_35</t>
   </si>
   <si>
-    <t>Unauthorised access</t>
-  </si>
-  <si>
-    <t>rename(embrace(p_11, p_63))</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Unauthorised access </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>in OEM and/or car services</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(embrace(p_63, p_11))</t>
   </si>
   <si>
     <t>f_36</t>
   </si>
   <si>
-    <t>embrace(p_25, p_45, p_51, p_58, p_74)</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Unreliable sources of information and/or rogue </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>car components</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(embrace(p_25, p_45, p_51, p_58, p_74))</t>
   </si>
   <si>
     <t>f_37</t>
@@ -728,10 +1004,40 @@
     <t>f_40</t>
   </si>
   <si>
+    <t>V2X message replay</t>
+  </si>
+  <si>
     <t>embrace(p_55, p_21, p_34, p_44)</t>
   </si>
   <si>
     <t>f_41</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Violation of rules and regulations/Breach of legislation/ Abuse of </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>driver</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> personal data</t>
+    </r>
+  </si>
+  <si>
+    <t>rename(p_28)</t>
   </si>
   <si>
     <t>Linkability</t>
@@ -1756,7 +2062,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.13"/>
-    <col customWidth="1" min="2" max="2" width="78.38"/>
+    <col customWidth="1" min="2" max="2" width="47.88"/>
     <col customWidth="1" min="3" max="3" width="8.88"/>
   </cols>
   <sheetData>
@@ -2615,7 +2921,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.13"/>
-    <col customWidth="1" min="2" max="2" width="78.38"/>
+    <col customWidth="1" min="2" max="2" width="47.25"/>
     <col customWidth="1" min="3" max="3" width="8.88"/>
     <col customWidth="1" min="4" max="10" width="5.13"/>
   </cols>
@@ -4401,8 +4707,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.5"/>
-    <col customWidth="1" min="2" max="2" width="60.75"/>
-    <col customWidth="1" min="3" max="3" width="43.5"/>
+    <col customWidth="1" min="2" max="2" width="70.0"/>
+    <col customWidth="1" min="3" max="3" width="41.38"/>
     <col customWidth="1" min="4" max="10" width="5.13"/>
   </cols>
   <sheetData>
@@ -4442,31 +4748,31 @@
       <c r="A2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="C2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -4480,7 +4786,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>129</v>
@@ -4502,13 +4808,13 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>163</v>
@@ -4530,16 +4836,16 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
@@ -4552,13 +4858,13 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>163</v>
@@ -4578,18 +4884,18 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -4606,18 +4912,18 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F9" s="9"/>
@@ -4630,16 +4936,16 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+        <v>187</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="8" t="s">
         <v>163</v>
       </c>
@@ -4650,7 +4956,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>137</v>
@@ -4670,7 +4976,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>121</v>
@@ -4690,7 +4996,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>55</v>
@@ -4712,16 +5018,16 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -4732,18 +5038,18 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="9"/>
       <c r="F15" s="8" t="s">
         <v>163</v>
       </c>
@@ -4754,16 +5060,16 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="9"/>
@@ -4776,16 +5082,16 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>163</v>
       </c>
@@ -4798,13 +5104,13 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>203</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>163</v>
@@ -4824,13 +5130,13 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>163</v>
@@ -4848,13 +5154,13 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -4868,7 +5174,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>61</v>
@@ -4888,18 +5194,18 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F22" s="9"/>
@@ -4914,18 +5220,18 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -4942,13 +5248,13 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>163</v>
@@ -4966,13 +5272,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>106</v>
+        <v>220</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>163</v>
@@ -4994,10 +5300,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>22</v>
@@ -5016,16 +5322,16 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F27" s="9"/>
@@ -5038,16 +5344,16 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+        <v>227</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="8" t="s">
@@ -5058,16 +5364,16 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+        <v>230</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="8" t="s">
@@ -5078,7 +5384,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>109</v>
@@ -5098,16 +5404,16 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="9"/>
@@ -5120,13 +5426,13 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -5140,18 +5446,18 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D33" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F33" s="8" t="s">
@@ -5170,18 +5476,18 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F34" s="8" t="s">
@@ -5198,13 +5504,13 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>163</v>
@@ -5220,18 +5526,18 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="8" t="s">
         <v>163</v>
@@ -5244,18 +5550,18 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D37" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F37" s="8" t="s">
@@ -5272,13 +5578,13 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>163</v>
@@ -5300,13 +5606,13 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -5320,13 +5626,13 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>163</v>
@@ -5344,13 +5650,13 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>115</v>
+        <v>259</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>163</v>
@@ -5372,16 +5678,16 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F42" s="9"/>
@@ -5411,13 +5717,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.63"/>
-    <col customWidth="1" min="2" max="2" width="22.88"/>
-    <col customWidth="1" min="3" max="3" width="17.63"/>
-    <col customWidth="1" min="4" max="4" width="22.13"/>
-    <col customWidth="1" min="5" max="5" width="22.38"/>
-    <col customWidth="1" min="6" max="6" width="34.13"/>
+    <col customWidth="1" min="2" max="2" width="12.38"/>
+    <col customWidth="1" min="3" max="3" width="12.5"/>
+    <col customWidth="1" min="4" max="4" width="10.25"/>
+    <col customWidth="1" min="5" max="5" width="15.5"/>
+    <col customWidth="1" min="6" max="6" width="11.25"/>
     <col customWidth="1" min="7" max="7" width="12.25"/>
-    <col customWidth="1" min="8" max="8" width="16.0"/>
+    <col customWidth="1" min="8" max="8" width="11.88"/>
     <col customWidth="1" min="9" max="9" width="21.25"/>
     <col customWidth="1" min="10" max="10" width="8.88"/>
     <col customWidth="1" min="11" max="11" width="12.75"/>
@@ -5428,67 +5734,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="12" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="12" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="12" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="12" t="s">
@@ -5496,230 +5802,230 @@
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="12" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="N2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>165</v>
       </c>
       <c r="K3" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>261</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="17" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="17" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="N4" s="17"/>
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="N5" s="17"/>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="17" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="N6" s="17"/>
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="17" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="17" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="18"/>
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="17" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="17" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="17" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
@@ -5728,27 +6034,27 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="14"/>
@@ -5758,23 +6064,23 @@
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="17" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="17" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="17" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="12" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
@@ -5784,28 +6090,28 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="17" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="17" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -5814,30 +6120,30 @@
     </row>
     <row r="12">
       <c r="A12" s="14" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="17" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -5846,28 +6152,28 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="17" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="14" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -5876,30 +6182,30 @@
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="17" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="14" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -5908,30 +6214,30 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="17" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="14" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -5940,28 +6246,28 @@
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="17" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="12" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="14" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -5970,28 +6276,28 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="14" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="17" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="17" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -6000,28 +6306,28 @@
     </row>
     <row r="18">
       <c r="A18" s="14" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="14" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="17" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="17" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -6030,27 +6336,27 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="17" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="17" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
@@ -6060,24 +6366,24 @@
     </row>
     <row r="20">
       <c r="A20" s="14" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="17" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -6086,28 +6392,28 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -6116,30 +6422,30 @@
     </row>
     <row r="22">
       <c r="A22" s="14" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="14" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -6148,24 +6454,24 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="12" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="17" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -6174,23 +6480,23 @@
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="14" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="17" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="12" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="14"/>
@@ -6200,26 +6506,26 @@
     </row>
     <row r="25">
       <c r="A25" s="14" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="17" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
@@ -6228,30 +6534,30 @@
     </row>
     <row r="26">
       <c r="A26" s="14" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
@@ -6260,23 +6566,23 @@
     </row>
     <row r="27">
       <c r="A27" s="14" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14" t="s">
-        <v>408</v>
+        <v>433</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -6286,23 +6592,23 @@
     </row>
     <row r="28">
       <c r="A28" s="14" t="s">
-        <v>409</v>
+        <v>434</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
@@ -6312,17 +6618,17 @@
     </row>
     <row r="29">
       <c r="A29" s="14" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
@@ -6334,17 +6640,17 @@
     </row>
     <row r="30">
       <c r="A30" s="14" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="14" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -6358,11 +6664,11 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="14" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -6378,13 +6684,13 @@
     </row>
     <row r="32">
       <c r="A32" s="17" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>424</v>
+        <v>449</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>425</v>
+        <v>450</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -6402,7 +6708,7 @@
       <c r="A33" s="18"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -6420,7 +6726,7 @@
       <c r="A34" s="14"/>
       <c r="B34" s="18"/>
       <c r="C34" s="14" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -6438,10 +6744,10 @@
       <c r="A35" s="14"/>
       <c r="B35" s="18"/>
       <c r="C35" s="14" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>429</v>
+        <v>454</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
@@ -6458,7 +6764,7 @@
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="14" t="s">
-        <v>430</v>
+        <v>455</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -6476,10 +6782,10 @@
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14" t="s">
-        <v>431</v>
+        <v>456</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>432</v>
+        <v>457</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -6496,7 +6802,7 @@
       <c r="A38" s="18"/>
       <c r="B38" s="14"/>
       <c r="C38" s="12" t="s">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="18"/>
@@ -6514,10 +6820,10 @@
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="17" t="s">
-        <v>434</v>
+        <v>459</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
@@ -6534,10 +6840,10 @@
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="17" t="s">
-        <v>435</v>
+        <v>460</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -6554,7 +6860,7 @@
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="17" t="s">
-        <v>437</v>
+        <v>462</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
@@ -6572,7 +6878,7 @@
       <c r="A42" s="14"/>
       <c r="B42" s="18"/>
       <c r="C42" s="17" t="s">
-        <v>438</v>
+        <v>463</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -6590,7 +6896,7 @@
       <c r="A43" s="14"/>
       <c r="B43" s="18"/>
       <c r="C43" s="17" t="s">
-        <v>439</v>
+        <v>464</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -6608,7 +6914,7 @@
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="17" t="s">
-        <v>440</v>
+        <v>465</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -21394,67 +21700,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="12" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="12" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="12" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="12" t="s">
@@ -21462,289 +21768,289 @@
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="12" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="N2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>165</v>
       </c>
       <c r="K3" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>261</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="17" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="17" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="N4" s="17"/>
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="N5" s="17"/>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="17" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="N6" s="17"/>
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="17" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="17" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>441</v>
+        <v>466</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="17" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="17" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="17" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="23" t="s">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="J9" s="17"/>
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="17" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="17" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="17" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="12" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="2"/>
@@ -21754,57 +22060,57 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="17" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="17" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="14" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="17" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -21813,28 +22119,28 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="17" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="14" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -21843,30 +22149,30 @@
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="17" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="14" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -21875,30 +22181,30 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="17" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="14" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -21907,28 +22213,28 @@
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="17" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="12" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="14" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -21937,28 +22243,28 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="14" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="17" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="17" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -21967,28 +22273,28 @@
     </row>
     <row r="18">
       <c r="A18" s="14" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="14" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="17" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="17" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -21997,27 +22303,27 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="17" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="17" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
@@ -22027,24 +22333,24 @@
     </row>
     <row r="20">
       <c r="A20" s="14" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="17" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -22053,28 +22359,28 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -22083,30 +22389,30 @@
     </row>
     <row r="22">
       <c r="A22" s="14" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="14" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -22115,24 +22421,24 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="12" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="17" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -22141,23 +22447,23 @@
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="14" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="17" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="12" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="14"/>
@@ -22167,26 +22473,26 @@
     </row>
     <row r="25">
       <c r="A25" s="14" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="17" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
@@ -22195,30 +22501,30 @@
     </row>
     <row r="26">
       <c r="A26" s="14" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
@@ -22227,23 +22533,23 @@
     </row>
     <row r="27">
       <c r="A27" s="14" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14" t="s">
-        <v>408</v>
+        <v>433</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -22253,23 +22559,23 @@
     </row>
     <row r="28">
       <c r="A28" s="14" t="s">
-        <v>409</v>
+        <v>434</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
@@ -22279,17 +22585,17 @@
     </row>
     <row r="29">
       <c r="A29" s="14" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
@@ -22300,17 +22606,17 @@
     </row>
     <row r="30">
       <c r="A30" s="14" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="14" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -22324,11 +22630,11 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="14" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -22344,13 +22650,13 @@
     </row>
     <row r="32">
       <c r="A32" s="17" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>424</v>
+        <v>449</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>425</v>
+        <v>450</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -22368,7 +22674,7 @@
       <c r="A33" s="18"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -22386,7 +22692,7 @@
       <c r="A34" s="14"/>
       <c r="B34" s="18"/>
       <c r="C34" s="14" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -22404,10 +22710,10 @@
       <c r="A35" s="14"/>
       <c r="B35" s="18"/>
       <c r="C35" s="14" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>429</v>
+        <v>454</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
@@ -22424,7 +22730,7 @@
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="14" t="s">
-        <v>430</v>
+        <v>455</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -22442,10 +22748,10 @@
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14" t="s">
-        <v>431</v>
+        <v>456</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>432</v>
+        <v>457</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -22462,7 +22768,7 @@
       <c r="A38" s="18"/>
       <c r="B38" s="14"/>
       <c r="C38" s="12" t="s">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="18"/>
@@ -22480,10 +22786,10 @@
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="17" t="s">
-        <v>434</v>
+        <v>459</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
@@ -22500,10 +22806,10 @@
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="17" t="s">
-        <v>435</v>
+        <v>460</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -22520,7 +22826,7 @@
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="17" t="s">
-        <v>437</v>
+        <v>462</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
@@ -22538,7 +22844,7 @@
       <c r="A42" s="14"/>
       <c r="B42" s="18"/>
       <c r="C42" s="17" t="s">
-        <v>438</v>
+        <v>463</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -22556,7 +22862,7 @@
       <c r="A43" s="14"/>
       <c r="B43" s="18"/>
       <c r="C43" s="17" t="s">
-        <v>439</v>
+        <v>464</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -22574,7 +22880,7 @@
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="17" t="s">
-        <v>440</v>
+        <v>465</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>

</xml_diff>